<commit_message>
add part b to the final report and also all csv needed for part c
</commit_message>
<xml_diff>
--- a/CSV/partB/MasterPartB.xlsx
+++ b/CSV/partB/MasterPartB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\choij\OneDrive\바탕 화면\SP2021\UOI\proj1\CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\choij\OneDrive\바탕 화면\SP2021\UOI\proj1\CSV\partB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E08FD4D-877B-4F03-8B19-4FB6376EB9C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D502484-7FB8-4408-B125-B5C4F85DE335}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8E21AE1F-41D4-4C4C-9F71-0BF9504DDDD2}"/>
   </bookViews>
@@ -18,16 +18,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">mostStudied_DataCovid!$A$2:$A$12</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">mostStudied_DataCovid!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">mostStudied_DataCovid!$B$2:$B$12</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">mostStudied_DataCovid!$A$2:$A$16</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">mostStudied_DataCovid!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">mostStudied_DataCovid!$B$2:$B$16</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">mostStudied_DataCovid!$A$1:$B$12</definedName>
     <definedName name="ExternalData_2" localSheetId="0" hidden="1">mostStudied_DataHepA!$A$1:$B$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -229,10 +224,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2099,16 +2091,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2147,34 +2139,12 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{F0D8E855-5DCC-4B84-B935-9E3A88686D04}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="3">
-    <queryTableFields count="2">
-      <queryTableField id="1" name="Column1" tableColumnId="1"/>
-      <queryTableField id="2" name="Column2" tableColumnId="2"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{55A8B1D2-1C5B-4F21-BCD2-E8A01FC8B4F9}" name="mostStudied_DataHepA" displayName="mostStudied_DataHepA" ref="A1:B15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B15" xr:uid="{72731735-042C-4998-9D5B-17ED6A0B6A98}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B440E930-95E8-4A96-8DC2-6983DCF590F2}" uniqueName="1" name="Drug" queryTableFieldId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{76522937-CBE8-4EDA-9854-483764FD0005}" uniqueName="2" name="Frequency" queryTableFieldId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6256676-973C-412D-AFC8-6C6C99FD7797}" name="mostStudied_DataCovid" displayName="mostStudied_DataCovid" ref="A1:B16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B16" xr:uid="{C9C763E9-AFBE-4DBA-9F70-B625C3AD9CF5}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EE9F56C3-C91B-4B1A-85E9-3AC10AFA5480}" uniqueName="1" name="Drug" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{CDDEF2FD-2F35-4D03-B2A1-0B320D0805C1}" uniqueName="2" name="Frequency" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2480,7 +2450,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,7 +2593,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2757,9 +2727,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>